<commit_message>
nearly finished the analysing part
 - plots nearly finished
- worked on the codebook
</commit_message>
<xml_diff>
--- a/plot assignment/Sova Mains.xlsx
+++ b/plot assignment/Sova Mains.xlsx
@@ -8,14 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tina\Documents\GitHub\dpm-assignments\plot assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97D2246F-3BF1-44E1-B42C-45234C7A1D28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{202AFBC7-3195-4B02-B8D7-E32EA4F47691}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sova1" sheetId="1" r:id="rId1"/>
     <sheet name="Sova2" sheetId="2" r:id="rId2"/>
-    <sheet name="combined" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="22">
   <si>
     <t>ID</t>
   </si>
@@ -89,7 +88,10 @@
     <t>Ascent</t>
   </si>
   <si>
-    <t>test</t>
+    <t>K/D</t>
+  </si>
+  <si>
+    <t>average Damage pro Round</t>
   </si>
 </sst>
 </file>
@@ -658,15 +660,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB3BF879-C4CD-4C90-90F0-FF757557EFE9}">
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection sqref="A1:K7"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -698,10 +700,13 @@
         <v>6</v>
       </c>
       <c r="K1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="L1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -733,7 +738,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -765,7 +770,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -797,7 +802,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -829,7 +834,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -861,7 +866,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -891,448 +896,6 @@
       </c>
       <c r="J7">
         <v>264</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA1F9C91-FA81-402F-AFDE-E4E1DB061967}">
-  <dimension ref="A1:K14"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N17" sqref="N17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>1</v>
-      </c>
-      <c r="H1" t="s">
-        <v>2</v>
-      </c>
-      <c r="I1" t="s">
-        <v>3</v>
-      </c>
-      <c r="J1" t="s">
-        <v>6</v>
-      </c>
-      <c r="K1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="1">
-        <v>45276</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2">
-        <v>21</v>
-      </c>
-      <c r="F2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2">
-        <v>17</v>
-      </c>
-      <c r="H2">
-        <v>12</v>
-      </c>
-      <c r="I2">
-        <v>5</v>
-      </c>
-      <c r="J2">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="1">
-        <v>45275</v>
-      </c>
-      <c r="C3">
-        <v>2</v>
-      </c>
-      <c r="D3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3">
-        <v>18</v>
-      </c>
-      <c r="F3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G3">
-        <v>18</v>
-      </c>
-      <c r="H3">
-        <v>9</v>
-      </c>
-      <c r="I3">
-        <v>6</v>
-      </c>
-      <c r="J3">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="1">
-        <v>45258</v>
-      </c>
-      <c r="C4">
-        <v>3</v>
-      </c>
-      <c r="D4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4">
-        <v>17</v>
-      </c>
-      <c r="F4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G4">
-        <v>20</v>
-      </c>
-      <c r="H4">
-        <v>10</v>
-      </c>
-      <c r="I4">
-        <v>3</v>
-      </c>
-      <c r="J4">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="1">
-        <v>45251</v>
-      </c>
-      <c r="C5">
-        <v>4</v>
-      </c>
-      <c r="D5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5">
-        <v>19</v>
-      </c>
-      <c r="F5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G5">
-        <v>18</v>
-      </c>
-      <c r="H5">
-        <v>15</v>
-      </c>
-      <c r="I5">
-        <v>6</v>
-      </c>
-      <c r="J5">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="1">
-        <v>45228</v>
-      </c>
-      <c r="C6">
-        <v>5</v>
-      </c>
-      <c r="D6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6">
-        <v>21</v>
-      </c>
-      <c r="F6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G6">
-        <v>16</v>
-      </c>
-      <c r="H6">
-        <v>16</v>
-      </c>
-      <c r="I6">
-        <v>6</v>
-      </c>
-      <c r="J6">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="1">
-        <v>45224</v>
-      </c>
-      <c r="C7">
-        <v>6</v>
-      </c>
-      <c r="D7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7">
-        <v>17</v>
-      </c>
-      <c r="F7" t="s">
-        <v>7</v>
-      </c>
-      <c r="G7">
-        <v>17</v>
-      </c>
-      <c r="H7">
-        <v>10</v>
-      </c>
-      <c r="I7">
-        <v>3</v>
-      </c>
-      <c r="J7">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="1">
-        <v>45262</v>
-      </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="D8" t="s">
-        <v>17</v>
-      </c>
-      <c r="E8">
-        <v>15</v>
-      </c>
-      <c r="F8" t="s">
-        <v>7</v>
-      </c>
-      <c r="G8">
-        <v>10</v>
-      </c>
-      <c r="H8">
-        <v>10</v>
-      </c>
-      <c r="I8">
-        <v>5</v>
-      </c>
-      <c r="J8">
-        <v>173</v>
-      </c>
-      <c r="K8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="1">
-        <v>45261</v>
-      </c>
-      <c r="C9">
-        <v>2</v>
-      </c>
-      <c r="D9" t="s">
-        <v>18</v>
-      </c>
-      <c r="E9">
-        <v>22</v>
-      </c>
-      <c r="F9" t="s">
-        <v>7</v>
-      </c>
-      <c r="G9">
-        <v>18</v>
-      </c>
-      <c r="H9">
-        <v>14</v>
-      </c>
-      <c r="I9">
-        <v>3</v>
-      </c>
-      <c r="J9">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="1">
-        <v>45261</v>
-      </c>
-      <c r="C10">
-        <v>3</v>
-      </c>
-      <c r="D10" t="s">
-        <v>17</v>
-      </c>
-      <c r="E10">
-        <v>23</v>
-      </c>
-      <c r="F10" t="s">
-        <v>8</v>
-      </c>
-      <c r="G10">
-        <v>22</v>
-      </c>
-      <c r="H10">
-        <v>15</v>
-      </c>
-      <c r="I10">
-        <v>7</v>
-      </c>
-      <c r="J10">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="1">
-        <v>45261</v>
-      </c>
-      <c r="C11">
-        <v>4</v>
-      </c>
-      <c r="D11" t="s">
-        <v>17</v>
-      </c>
-      <c r="E11">
-        <v>17</v>
-      </c>
-      <c r="F11" t="s">
-        <v>8</v>
-      </c>
-      <c r="G11">
-        <v>13</v>
-      </c>
-      <c r="H11">
-        <v>13</v>
-      </c>
-      <c r="I11">
-        <v>4</v>
-      </c>
-      <c r="J11">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" s="1">
-        <v>45256</v>
-      </c>
-      <c r="C12">
-        <v>5</v>
-      </c>
-      <c r="D12" t="s">
-        <v>19</v>
-      </c>
-      <c r="E12">
-        <v>18</v>
-      </c>
-      <c r="F12" t="s">
-        <v>8</v>
-      </c>
-      <c r="G12">
-        <v>7</v>
-      </c>
-      <c r="H12">
-        <v>13</v>
-      </c>
-      <c r="I12">
-        <v>2</v>
-      </c>
-      <c r="J12">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13" s="1">
-        <v>45256</v>
-      </c>
-      <c r="C13">
-        <v>6</v>
-      </c>
-      <c r="D13" t="s">
-        <v>19</v>
-      </c>
-      <c r="E13">
-        <v>22</v>
-      </c>
-      <c r="F13" t="s">
-        <v>8</v>
-      </c>
-      <c r="G13">
-        <v>14</v>
-      </c>
-      <c r="H13">
-        <v>15</v>
-      </c>
-      <c r="I13">
-        <v>8</v>
-      </c>
-      <c r="J13">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="K14" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>